<commit_message>
add result of prompt2
</commit_message>
<xml_diff>
--- a/data/new_novel_need.xlsx
+++ b/data/new_novel_need.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/lichunhao/Dropbox/Work/恒生RA/novel need/src/data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/chunhaoli/Documents/Work/novel_need/novel-need-detection/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0252C4A3-B265-A44D-8868-9B24BDB706B0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B591D9AB-B2CB-3D4A-B2E1-F266F12931D8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="700" windowWidth="27040" windowHeight="15420" xr2:uid="{2094ED5C-6790-0C46-B56A-E0F9759D3B47}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="345" uniqueCount="266">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="346" uniqueCount="267">
   <si>
     <t>If AORUS offers two AC adapters to end user will be fantastic!!</t>
   </si>
@@ -827,23 +827,27 @@
   </si>
   <si>
     <t>The graphics card on this device is removable, allowing me to upgrade to a more powerful one in the future. It's a feature that's ensured the device's future-proofing, making it a great investment.</t>
+  </si>
+  <si>
+    <t>generate_v1</t>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="6">
     <font>
       <sz val="12"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="等线"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="9"/>
-      <name val="Calibri"/>
+      <name val="等线"/>
       <family val="3"/>
       <charset val="134"/>
       <scheme val="minor"/>
@@ -916,7 +920,7 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="常规" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -932,7 +936,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 主题​​">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -1228,18 +1232,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E6697C36-D247-DE4E-9635-E653A91D407D}">
-  <dimension ref="A1:E81"/>
+  <dimension ref="A1:F81"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A36" zoomScale="93" workbookViewId="0">
-      <selection activeCell="B48" sqref="B48"/>
+    <sheetView tabSelected="1" zoomScale="93" workbookViewId="0">
+      <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="16"/>
   <cols>
     <col min="1" max="1" width="123.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:6">
       <c r="A1" s="1" t="s">
         <v>6</v>
       </c>
@@ -1255,8 +1259,11 @@
       <c r="E1" t="s">
         <v>125</v>
       </c>
-    </row>
-    <row r="2" spans="1:5" ht="20" x14ac:dyDescent="0.2">
+      <c r="F1" t="s">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" ht="20">
       <c r="A2" s="1" t="s">
         <v>76</v>
       </c>
@@ -1273,7 +1280,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="3" spans="1:5" ht="20" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:6" ht="20">
       <c r="A3" s="1" t="s">
         <v>72</v>
       </c>
@@ -1290,7 +1297,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="4" spans="1:5" ht="20" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:6" ht="20">
       <c r="A4" s="1" t="s">
         <v>73</v>
       </c>
@@ -1307,7 +1314,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="5" spans="1:5" ht="20" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:6" ht="20">
       <c r="A5" s="1" t="s">
         <v>74</v>
       </c>
@@ -1324,7 +1331,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="6" spans="1:5" ht="20" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:6" ht="20">
       <c r="A6" s="1" t="s">
         <v>75</v>
       </c>
@@ -1341,7 +1348,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="7" spans="1:5" ht="20" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:6" ht="20">
       <c r="A7" s="1" t="s">
         <v>77</v>
       </c>
@@ -1358,7 +1365,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="8" spans="1:5" ht="20" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:6" ht="20">
       <c r="A8" s="2" t="s">
         <v>78</v>
       </c>
@@ -1375,7 +1382,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="9" spans="1:5" ht="20" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:6" ht="20">
       <c r="A9" s="2" t="s">
         <v>79</v>
       </c>
@@ -1392,7 +1399,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="10" spans="1:5" ht="20" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:6" ht="20">
       <c r="A10" s="2" t="s">
         <v>80</v>
       </c>
@@ -1409,7 +1416,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="11" spans="1:5" ht="20" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:6" ht="20">
       <c r="A11" s="2" t="s">
         <v>81</v>
       </c>
@@ -1426,7 +1433,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="12" spans="1:5" ht="20" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:6" ht="20">
       <c r="A12" s="2" t="s">
         <v>82</v>
       </c>
@@ -1443,7 +1450,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="13" spans="1:5" ht="20" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:6" ht="20">
       <c r="A13" s="2" t="s">
         <v>0</v>
       </c>
@@ -1460,7 +1467,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="14" spans="1:5" ht="20" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:6" ht="20">
       <c r="A14" s="3" t="s">
         <v>1</v>
       </c>
@@ -1477,7 +1484,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="15" spans="1:5" ht="20" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:6" ht="20">
       <c r="A15" s="1" t="s">
         <v>2</v>
       </c>
@@ -1494,7 +1501,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="16" spans="1:5" ht="20" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:6" ht="20">
       <c r="A16" s="1" t="s">
         <v>3</v>
       </c>
@@ -1511,7 +1518,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="17" spans="1:5" ht="20" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:5" ht="20">
       <c r="A17" s="1" t="s">
         <v>4</v>
       </c>
@@ -1528,7 +1535,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="18" spans="1:5" ht="20" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:5" ht="20">
       <c r="A18" s="1" t="s">
         <v>5</v>
       </c>
@@ -1545,7 +1552,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="19" spans="1:5" ht="20" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:5" ht="20">
       <c r="A19" s="1" t="s">
         <v>7</v>
       </c>
@@ -1562,7 +1569,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="20" spans="1:5" ht="20" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:5" ht="20">
       <c r="A20" s="1" t="s">
         <v>8</v>
       </c>
@@ -1579,7 +1586,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="21" spans="1:5" ht="20" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:5" ht="20">
       <c r="A21" s="1" t="s">
         <v>9</v>
       </c>
@@ -1596,7 +1603,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="22" spans="1:5" ht="20" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:5" ht="20">
       <c r="A22" s="1" t="s">
         <v>10</v>
       </c>
@@ -1610,7 +1617,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="23" spans="1:5" ht="20" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:5" ht="20">
       <c r="A23" s="1" t="s">
         <v>11</v>
       </c>
@@ -1624,7 +1631,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="24" spans="1:5" ht="20" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:5" ht="20">
       <c r="A24" s="1" t="s">
         <v>12</v>
       </c>
@@ -1638,7 +1645,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="25" spans="1:5" ht="20" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:5" ht="20">
       <c r="A25" s="1" t="s">
         <v>13</v>
       </c>
@@ -1652,7 +1659,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="26" spans="1:5" ht="20" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:5" ht="20">
       <c r="A26" s="1" t="s">
         <v>14</v>
       </c>
@@ -1666,7 +1673,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="27" spans="1:5" ht="20" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:5" ht="20">
       <c r="A27" s="1" t="s">
         <v>15</v>
       </c>
@@ -1680,7 +1687,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="28" spans="1:5" ht="20" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:5" ht="20">
       <c r="A28" s="1" t="s">
         <v>16</v>
       </c>
@@ -1694,7 +1701,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="29" spans="1:5" ht="20" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:5" ht="20">
       <c r="A29" s="1" t="s">
         <v>17</v>
       </c>
@@ -1708,7 +1715,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="30" spans="1:5" ht="20" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:5" ht="20">
       <c r="A30" s="1" t="s">
         <v>18</v>
       </c>
@@ -1722,7 +1729,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="31" spans="1:5" ht="20" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:5" ht="20">
       <c r="A31" s="1" t="s">
         <v>19</v>
       </c>
@@ -1736,7 +1743,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="32" spans="1:5" ht="20" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:5" ht="20">
       <c r="A32" s="1" t="s">
         <v>20</v>
       </c>
@@ -1750,7 +1757,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="33" spans="1:4" ht="20" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:4" ht="20">
       <c r="A33" s="1" t="s">
         <v>21</v>
       </c>
@@ -1764,7 +1771,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="34" spans="1:4" ht="20" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:4" ht="20">
       <c r="A34" s="1" t="s">
         <v>22</v>
       </c>
@@ -1778,7 +1785,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="35" spans="1:4" ht="20" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:4" ht="20">
       <c r="A35" s="1" t="s">
         <v>23</v>
       </c>
@@ -1792,7 +1799,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="36" spans="1:4" ht="20" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:4" ht="20">
       <c r="A36" s="1" t="s">
         <v>24</v>
       </c>
@@ -1806,7 +1813,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="37" spans="1:4" ht="20" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:4" ht="20">
       <c r="A37" s="1" t="s">
         <v>25</v>
       </c>
@@ -1820,7 +1827,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="38" spans="1:4" ht="20" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:4" ht="20">
       <c r="A38" s="1" t="s">
         <v>26</v>
       </c>
@@ -1834,7 +1841,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="39" spans="1:4" ht="20" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:4" ht="20">
       <c r="A39" s="1" t="s">
         <v>27</v>
       </c>
@@ -1848,7 +1855,7 @@
         <v>163</v>
       </c>
     </row>
-    <row r="40" spans="1:4" ht="20" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:4" ht="20">
       <c r="A40" s="1" t="s">
         <v>28</v>
       </c>
@@ -1862,7 +1869,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="41" spans="1:4" ht="20" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:4" ht="20">
       <c r="A41" s="1" t="s">
         <v>29</v>
       </c>
@@ -1876,7 +1883,7 @@
         <v>165</v>
       </c>
     </row>
-    <row r="42" spans="1:4" ht="20" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:4" ht="20">
       <c r="A42" s="1" t="s">
         <v>30</v>
       </c>
@@ -1890,7 +1897,7 @@
         <v>226</v>
       </c>
     </row>
-    <row r="43" spans="1:4" ht="20" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:4" ht="20">
       <c r="A43" s="1" t="s">
         <v>31</v>
       </c>
@@ -1904,7 +1911,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="44" spans="1:4" ht="20" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:4" ht="20">
       <c r="A44" s="1" t="s">
         <v>32</v>
       </c>
@@ -1918,7 +1925,7 @@
         <v>228</v>
       </c>
     </row>
-    <row r="45" spans="1:4" ht="20" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:4" ht="20">
       <c r="A45" s="1" t="s">
         <v>33</v>
       </c>
@@ -1932,7 +1939,7 @@
         <v>229</v>
       </c>
     </row>
-    <row r="46" spans="1:4" ht="20" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:4" ht="20">
       <c r="A46" s="1" t="s">
         <v>34</v>
       </c>
@@ -1946,7 +1953,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="47" spans="1:4" ht="20" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:4" ht="20">
       <c r="A47" s="1" t="s">
         <v>35</v>
       </c>
@@ -1960,7 +1967,7 @@
         <v>231</v>
       </c>
     </row>
-    <row r="48" spans="1:4" ht="20" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:4" ht="20">
       <c r="A48" s="1" t="s">
         <v>36</v>
       </c>
@@ -1974,7 +1981,7 @@
         <v>232</v>
       </c>
     </row>
-    <row r="49" spans="1:4" ht="20" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:4" ht="20">
       <c r="A49" s="1" t="s">
         <v>37</v>
       </c>
@@ -1988,7 +1995,7 @@
         <v>233</v>
       </c>
     </row>
-    <row r="50" spans="1:4" ht="20" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:4" ht="20">
       <c r="A50" s="1" t="s">
         <v>38</v>
       </c>
@@ -2002,7 +2009,7 @@
         <v>234</v>
       </c>
     </row>
-    <row r="51" spans="1:4" ht="20" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:4" ht="20">
       <c r="A51" s="1" t="s">
         <v>39</v>
       </c>
@@ -2016,7 +2023,7 @@
         <v>235</v>
       </c>
     </row>
-    <row r="52" spans="1:4" ht="20" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:4" ht="20">
       <c r="A52" s="1" t="s">
         <v>40</v>
       </c>
@@ -2030,7 +2037,7 @@
         <v>236</v>
       </c>
     </row>
-    <row r="53" spans="1:4" ht="20" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:4" ht="20">
       <c r="A53" s="1" t="s">
         <v>41</v>
       </c>
@@ -2044,7 +2051,7 @@
         <v>237</v>
       </c>
     </row>
-    <row r="54" spans="1:4" ht="20" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:4" ht="20">
       <c r="A54" s="1" t="s">
         <v>42</v>
       </c>
@@ -2058,7 +2065,7 @@
         <v>238</v>
       </c>
     </row>
-    <row r="55" spans="1:4" ht="20" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:4" ht="20">
       <c r="A55" s="1" t="s">
         <v>43</v>
       </c>
@@ -2072,7 +2079,7 @@
         <v>239</v>
       </c>
     </row>
-    <row r="56" spans="1:4" ht="20" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:4" ht="20">
       <c r="A56" s="1" t="s">
         <v>44</v>
       </c>
@@ -2086,7 +2093,7 @@
         <v>240</v>
       </c>
     </row>
-    <row r="57" spans="1:4" ht="20" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:4" ht="20">
       <c r="A57" s="1" t="s">
         <v>45</v>
       </c>
@@ -2100,7 +2107,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="58" spans="1:4" ht="20" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:4" ht="20">
       <c r="A58" s="1" t="s">
         <v>46</v>
       </c>
@@ -2114,7 +2121,7 @@
         <v>242</v>
       </c>
     </row>
-    <row r="59" spans="1:4" ht="20" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:4" ht="20">
       <c r="A59" s="1" t="s">
         <v>47</v>
       </c>
@@ -2128,7 +2135,7 @@
         <v>243</v>
       </c>
     </row>
-    <row r="60" spans="1:4" ht="20" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:4" ht="20">
       <c r="A60" s="1" t="s">
         <v>48</v>
       </c>
@@ -2142,7 +2149,7 @@
         <v>244</v>
       </c>
     </row>
-    <row r="61" spans="1:4" ht="20" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:4" ht="20">
       <c r="A61" s="1" t="s">
         <v>49</v>
       </c>
@@ -2156,7 +2163,7 @@
         <v>245</v>
       </c>
     </row>
-    <row r="62" spans="1:4" ht="20" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:4" ht="20">
       <c r="A62" s="1" t="s">
         <v>50</v>
       </c>
@@ -2170,7 +2177,7 @@
         <v>246</v>
       </c>
     </row>
-    <row r="63" spans="1:4" ht="20" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:4" ht="20">
       <c r="A63" s="1" t="s">
         <v>51</v>
       </c>
@@ -2184,7 +2191,7 @@
         <v>247</v>
       </c>
     </row>
-    <row r="64" spans="1:4" ht="20" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:4" ht="20">
       <c r="A64" s="1" t="s">
         <v>52</v>
       </c>
@@ -2198,7 +2205,7 @@
         <v>248</v>
       </c>
     </row>
-    <row r="65" spans="1:4" ht="20" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:4" ht="20">
       <c r="A65" s="1" t="s">
         <v>53</v>
       </c>
@@ -2212,7 +2219,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="66" spans="1:4" ht="20" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:4" ht="20">
       <c r="A66" s="1" t="s">
         <v>54</v>
       </c>
@@ -2226,7 +2233,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="67" spans="1:4" ht="20" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:4" ht="20">
       <c r="A67" s="1" t="s">
         <v>55</v>
       </c>
@@ -2240,7 +2247,7 @@
         <v>251</v>
       </c>
     </row>
-    <row r="68" spans="1:4" ht="20" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:4" ht="20">
       <c r="A68" s="1" t="s">
         <v>56</v>
       </c>
@@ -2254,7 +2261,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="69" spans="1:4" ht="20" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:4" ht="20">
       <c r="A69" s="1" t="s">
         <v>57</v>
       </c>
@@ -2268,7 +2275,7 @@
         <v>253</v>
       </c>
     </row>
-    <row r="70" spans="1:4" ht="20" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:4" ht="20">
       <c r="A70" s="1" t="s">
         <v>58</v>
       </c>
@@ -2282,7 +2289,7 @@
         <v>254</v>
       </c>
     </row>
-    <row r="71" spans="1:4" ht="20" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:4" ht="20">
       <c r="A71" s="1" t="s">
         <v>59</v>
       </c>
@@ -2296,7 +2303,7 @@
         <v>255</v>
       </c>
     </row>
-    <row r="72" spans="1:4" ht="20" x14ac:dyDescent="0.2">
+    <row r="72" spans="1:4" ht="20">
       <c r="A72" s="1" t="s">
         <v>60</v>
       </c>
@@ -2310,7 +2317,7 @@
         <v>256</v>
       </c>
     </row>
-    <row r="73" spans="1:4" ht="20" x14ac:dyDescent="0.2">
+    <row r="73" spans="1:4" ht="20">
       <c r="A73" s="1" t="s">
         <v>61</v>
       </c>
@@ -2324,7 +2331,7 @@
         <v>257</v>
       </c>
     </row>
-    <row r="74" spans="1:4" ht="20" x14ac:dyDescent="0.2">
+    <row r="74" spans="1:4" ht="20">
       <c r="A74" s="1" t="s">
         <v>62</v>
       </c>
@@ -2338,7 +2345,7 @@
         <v>258</v>
       </c>
     </row>
-    <row r="75" spans="1:4" ht="20" x14ac:dyDescent="0.2">
+    <row r="75" spans="1:4" ht="20">
       <c r="A75" s="1" t="s">
         <v>63</v>
       </c>
@@ -2352,7 +2359,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="76" spans="1:4" ht="20" x14ac:dyDescent="0.2">
+    <row r="76" spans="1:4" ht="20">
       <c r="A76" s="1" t="s">
         <v>64</v>
       </c>
@@ -2366,7 +2373,7 @@
         <v>260</v>
       </c>
     </row>
-    <row r="77" spans="1:4" ht="20" x14ac:dyDescent="0.2">
+    <row r="77" spans="1:4" ht="20">
       <c r="A77" s="1" t="s">
         <v>65</v>
       </c>
@@ -2380,7 +2387,7 @@
         <v>261</v>
       </c>
     </row>
-    <row r="78" spans="1:4" ht="20" x14ac:dyDescent="0.2">
+    <row r="78" spans="1:4" ht="20">
       <c r="A78" s="1" t="s">
         <v>66</v>
       </c>
@@ -2394,7 +2401,7 @@
         <v>262</v>
       </c>
     </row>
-    <row r="79" spans="1:4" ht="20" x14ac:dyDescent="0.2">
+    <row r="79" spans="1:4" ht="20">
       <c r="A79" s="1" t="s">
         <v>67</v>
       </c>
@@ -2408,7 +2415,7 @@
         <v>263</v>
       </c>
     </row>
-    <row r="80" spans="1:4" ht="20" x14ac:dyDescent="0.2">
+    <row r="80" spans="1:4" ht="20">
       <c r="A80" s="1" t="s">
         <v>68</v>
       </c>
@@ -2422,7 +2429,7 @@
         <v>264</v>
       </c>
     </row>
-    <row r="81" spans="1:4" ht="20" x14ac:dyDescent="0.2">
+    <row r="81" spans="1:4" ht="20">
       <c r="A81" s="1" t="s">
         <v>69</v>
       </c>

</xml_diff>

<commit_message>
update new novel need
</commit_message>
<xml_diff>
--- a/data/new_novel_need.xlsx
+++ b/data/new_novel_need.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/chunhaoli/Documents/Work/novel_need/novel-need-detection/data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/lichunhao/Dropbox/Work/恒生RA/novel need/src/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B591D9AB-B2CB-3D4A-B2E1-F266F12931D8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8BB5A603-8F53-CA46-B569-C9B5D91F974D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="700" windowWidth="27040" windowHeight="15420" xr2:uid="{2094ED5C-6790-0C46-B56A-E0F9759D3B47}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="346" uniqueCount="267">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="426" uniqueCount="344">
   <si>
     <t>If AORUS offers two AC adapters to end user will be fantastic!!</t>
   </si>
@@ -831,23 +831,254 @@
   <si>
     <t>generate_v1</t>
     <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>I think this computer is overall not bad, and the cooling is okay, but I hope it can add a voice assistant that can help me automatically find files and clean up junk, which would be more convenient.</t>
+  </si>
+  <si>
+    <t>The computer runs fast, but the cooling is lacking. It would be great if it could use a freeze-like technology to cool down in a second. And then there is the screen quality is not good, cracks appeared without much use.</t>
+  </si>
+  <si>
+    <t>This computer has a great processing speed and the design is sleek, but the battery life leaves a lot to be desired. I hope in the future they could incorporate solar charging features so I could work all day without worrying about running out of power.</t>
+  </si>
+  <si>
+    <t>The graphics card on this machine is top-notch, excellent for gaming. However, the speakers could use a boost. It would be fantastic if they added surround sound capabilities, to immerse you in the gaming experience fully.</t>
+  </si>
+  <si>
+    <t>I'm quite satisfied with the storage capacity of this computer, but the keyboard is a bit clunky. I wish they would develop a holographic keyboard that adjusts to your typing style for an even more personalized experience.</t>
+  </si>
+  <si>
+    <t>This computer's compact size is perfect for traveling, but the webcam quality is poor. I dream of the day when they install 4K resolution webcams for crystal clear video calls.</t>
+  </si>
+  <si>
+    <t>I adore the fast boot time on this machine, but the customer service was underwhelming when I had an issue. If only the computer could have a built-in diagnostic tool that could troubleshoot and fix problems automatically!</t>
+  </si>
+  <si>
+    <t>The display on this computer is stunning, but the touchpad feels a bit outdated. I'd love it if they could integrate gesture recognition technology for a seamless and intuitive navigation experience.</t>
+  </si>
+  <si>
+    <t>This machine's value for money is fantastic, but the lack of port options is disappointing. It would be a game-changer if they could include a universal port that could accommodate any type of cable or accessory.</t>
+  </si>
+  <si>
+    <t>I'm impressed with the durability of this computer, but the noise of the fan can be a bit distracting. I wish they would invent a silent cooling system that could keep the computer cool without a sound.</t>
+  </si>
+  <si>
+    <t>This computer is user-friendly and easy to set up, but the weight is a little too much for my liking. If they could use lighter materials without compromising on durability, that would be perfect.</t>
+  </si>
+  <si>
+    <t>The software compatibility of this computer is excellent, but the color accuracy of the screen is mediocre. I hope they will incorporate OLED technology for a more vibrant and true-to-life color representation.</t>
+  </si>
+  <si>
+    <t>I'm genuinely pleased with the security features on this computer, from the fingerprint reader to the end-to-end encryption. However, the one thing that's missing is an AI-powered facial recognition system that can automatically lock the computer when it detects an unfamiliar face.</t>
+  </si>
+  <si>
+    <t>The sleek aesthetics of this computer are impressive, but the hinges feel a bit flimsy. My dream would be to have a liquid metal hinge that adjusts to any angle while maintaining a sturdy and firm hold.</t>
+  </si>
+  <si>
+    <t>The speed and power of this machine are truly commendable, but I feel like the power consumption is too high. It would be a game-changer if they could invent an energy-efficient system that harnesses kinetic energy from the keyboard and mouse movements.</t>
+  </si>
+  <si>
+    <t>The pre-installed software on this computer is helpful, but the bloatware is a nuisance. An innovative idea would be an intelligent software manager that can automatically detect and uninstall unwanted programs.</t>
+  </si>
+  <si>
+    <t>The precision of the touch screen on this computer is quite good, but I can't help but wish for a 3D holographic display that I could manipulate with hand gestures, like in those sci-fi movies.</t>
+  </si>
+  <si>
+    <t>I appreciate the high-quality audio of the speakers on this computer, but the lack of noise cancellation can be a downside during video calls. A futuristic feature would be an AI-powered noise cancellation system that can differentiate between voice and background noise.</t>
+  </si>
+  <si>
+    <t>The seamless integration with my other devices is a definite advantage, but the Bluetooth connection sometimes drops out. I dream of a world where the computer has a self-healing wireless system that can troubleshoot and repair its connection issues.</t>
+  </si>
+  <si>
+    <t>The keyboard layout of this computer is pretty intuitive, but the lack of backlighting makes it hard to use in dimly lit conditions. A feature I would love to see is smart keyboard lighting that adjusts based on the room's light conditions.</t>
+  </si>
+  <si>
+    <t>This computer's robustness and resistance to damage is commendable, but the exterior finish is prone to scratches. I imagine a future where they use self-healing materials that can repair minor scratches and keep the machine looking brand new.</t>
+  </si>
+  <si>
+    <t>I'm quite impressed with the variety of ports on this computer, but the lack of a dedicated microSD slot can be inconvenient. It would be revolutionary if they could design a multi-function port that could morph to accommodate any type of connector.</t>
+  </si>
+  <si>
+    <t>Upon unboxing this computer, I was immediately struck by its sophisticated design and the cool, metallic feel of its casing. However, the screen, while offering decent resolution, lacks the vibrancy I have experienced in other models. If only it were possible for them to integrate dynamic color calibration, which would adjust the display based on ambient light conditions and the color palette of the content being viewed - this could truly revolutionize the user experience!</t>
+  </si>
+  <si>
+    <t>The impressive computational power and speed of this computer are undeniable. It handles heavy-duty software without breaking a sweat. However, the battery life leaves a lot to be desired, barely lasting through half a day of work. How revolutionary would it be to have a self-charging feature that harnesses thermal energy from the device's heat output, converting it into power?</t>
+  </si>
+  <si>
+    <t>This computer's large storage capacity and fast read-write speeds are truly commendable, making file transfers a breeze. Unfortunately, the sound system does not match up. The speakers are tinny and lack depth. If they were to introduce a feature that creates a virtual surround sound experience, it would be a massive leap forward in enhancing multimedia consumption.</t>
+  </si>
+  <si>
+    <t>I must commend the manufacturers for the seamless integration between this computer and other devices in the ecosystem. However, the video calling experience is subpar due to the average webcam quality. I envision a future where the computer comes with an AI-assisted camera that adjusts focus and lighting conditions in real-time, guaranteeing a professional video call experience.</t>
+  </si>
+  <si>
+    <t>Despite the sleek and stylish exterior, the computer's weight is a bit on the higher side, making portability an issue. I would love to see them use graphene or some other lightweight, durable material in the future. Imagine a computer so light, you'd barely feel it in your backpack!</t>
+  </si>
+  <si>
+    <t>The keyboard on this computer is spacious and comfortable, but the lack of a dedicated numeric keypad is a drawback for someone who works a lot with numbers. I hope that one day we'll see a flexible OLED touchpad that could morph into a numeric keypad or a drawing pad based on the user's needs.</t>
+  </si>
+  <si>
+    <t>The built-in security features, including the fingerprint reader and encryption software, are top-notch. However, I would love to see more personalized security features, like a voice recognition system that can identify the user based on their unique speech patterns and even detect stress levels to identify potential security threats.</t>
+  </si>
+  <si>
+    <t>While the computer boasts of a high-quality display and excellent sound system, the lack of immersive features for gaming is a downside. I dream of the day when computers come with built-in VR capabilities that could transform any game into an immersive experience without the need for additional hardware.</t>
+  </si>
+  <si>
+    <t>The customer service experience was prompt and efficient when I faced a minor issue with the computer. However, I wish there was a more personalized approach, like a dedicated AI customer service assistant for each user, capable of predicting and solving issues even before the user notices them.</t>
+  </si>
+  <si>
+    <t>The durability of this computer is quite impressive, withstanding everyday wear and tear without a hitch. However, the exterior gets quite smudgy and requires constant cleaning. I imagine a future where the computer's surface has a self-cleaning feature, using nano-technology to repel dust and stains.</t>
+  </si>
+  <si>
+    <t>Opening up this computer was like love at first sight. Its sleek lines and futuristic design were absolutely breathtaking. However, the fan noise drives me up the wall! It’s like having a mini jet engine on my desk. If only they could develop a soundproof casing or a fanless cooling system, that would be a real game-changer!</t>
+  </si>
+  <si>
+    <t>I am genuinely thrilled by this computer's speedy boot-up time, it's practically instantaneous! But, when it comes to the battery life, it's a whole different ballgame. It’s utterly frustrating to have to constantly worry about carrying my charger around. I long for the day when they will incorporate a regenerative power system that uses the computer's heat or even kinetic energy from typing to charge the battery.</t>
+  </si>
+  <si>
+    <t>The graphics on this machine are simply out of this world, making my gaming sessions incredibly immersive. However, the keyboard leaves much to be desired, with the keys feeling mushy and unresponsive. I dream of the day when they integrate haptic feedback into the keyboard, providing a tactile response to every keypress.</t>
+  </si>
+  <si>
+    <t>I've got to hand it to them, the processing power of this computer is nothing short of awe-inspiring, handling multiple resource-intensive tasks with ease. But, I can't help but groan at the lack of customization options in the settings. How amazing would it be if they could include an AI assistant that can learn my preferences and automatically adjust the settings accordingly?</t>
+  </si>
+  <si>
+    <t>The pre-installed software suite on this computer is highly functional and user-friendly, but the number of unnecessary apps is mind-boggling. It would be fantastic if there was an intelligent system that could recognize rarely used programs and suggest their removal to free up system resources.</t>
+  </si>
+  <si>
+    <t>The high-resolution display of this computer is a sight for sore eyes, offering an incredibly crisp and vibrant viewing experience. However, the speakers are so tinny and hollow that they totally ruin the multimedia experience. My hope is that they will include a virtual surround sound feature in future models, to make movies and music come alive.</t>
+  </si>
+  <si>
+    <t>This computer's compatibility with a wide range of peripherals is truly impressive, but the arrangement of the ports is quite annoying. How about a modular port system that allows users to rearrange the ports according to their personal preferences?</t>
+  </si>
+  <si>
+    <t>The customer support for this computer was helpful and responsive, but I dread the thought of going through the whole process again if I run into another problem. I would be over the moon if they could develop an integrated self-diagnosis tool that can automatically detect issues and offer real-time solutions.</t>
+  </si>
+  <si>
+    <t>The solid build quality of this computer inspires confidence, but the weight is a real workout for my arms when I have to lug it around. Imagine a future where they could use advanced, lightweight materials to make the computer as light as a feather without compromising on durability.</t>
+  </si>
+  <si>
+    <t>The Wi-Fi connectivity of this computer is pretty solid, but the lack of an Ethernet port is a real headache when I need a stable connection for critical tasks. How revolutionary would it be if they could introduce a universal wireless system that could offer the same stability and speed as a wired connection?</t>
+  </si>
+  <si>
+    <t>The moment I laid eyes on this computer, I was smitten by its sleek, polished look. But oh, the heartbreak when I realized the glossy finish is a magnet for fingerprints! I yearn for the day when they'll use some sort of fingerprint-resistant coating to keep it looking pristine all the time.</t>
+  </si>
+  <si>
+    <t>This computer's speed is like a dream come true, it's as swift as a cheetah. But, oh the agony when I have to use the touchpad! It's so unresponsive, it's like trying to stir molasses. I wish they could invent a touchpad with haptic feedback to give a tangible response to every swipe and click.</t>
+  </si>
+  <si>
+    <t>The clarity of the display on this computer is a real feast for the eyes, with vivid colors and sharp lines. However, the built-in speakers are a real letdown, sounding more like a tin can than a quality audio system. It would be incredible if they could integrate a spatial audio system to make the sound feel as immersive as the visuals.</t>
+  </si>
+  <si>
+    <t>The storage space on this computer is impressive, it's like having a warehouse at my disposal. But, it's a real headache when I try to find an old file. How amazing would it be if they could develop a smart filing system that organizes and tags files based on their content?</t>
+  </si>
+  <si>
+    <t>This computer's compatibility with other devices is truly remarkable, it's like a universal translator for technology. However, the weight is a real deal-breaker, it's like carrying around a brick. I can't wait for the day when they'll incorporate advanced, lightweight materials, making the computer as light as a feather.</t>
+  </si>
+  <si>
+    <t>The keyboard on this computer is a joy to use, with a comfortable layout and satisfying key travel. But the battery life? It's absolutely pitiful. It feels like I'm forever tethered to a power outlet. I hope they can pioneer a battery technology that charges from ambient light, freeing me from the chains of the charger.</t>
+  </si>
+  <si>
+    <t>The cooling system on this computer is top-notch, it runs as cool as a cucumber even under heavy load. But the glossy screen is a nightmare in bright light, it's like looking into a mirror. I long for a matte screen option that eliminates glare and allows me to work anywhere I want.</t>
+  </si>
+  <si>
+    <t>The processing power of this computer is awe-inspiring, it devours complex tasks like a beast. But the fan noise is a real distraction, it sounds like a swarm of bees in my ear. I would be overjoyed if they could develop a whisper-quiet cooling system that keeps the peace and quiet.</t>
+  </si>
+  <si>
+    <t>This computer's robust build quality is truly impressive, it feels like it could survive a fall off a cliff. But the lack of a touchscreen is a real disappointment, it's like driving a car without power steering. I'm looking forward to the day when they'll introduce a responsive touchscreen that makes navigation a breeze.</t>
+  </si>
+  <si>
+    <t>The Wi-Fi connectivity on this computer is rock solid, it's as reliable as a loyal friend. However, the limited USB ports are a real inconvenience, it's like trying to fit a quart into a pint pot. I dream of a future where they'll include a modular port system that lets me add the ports I need.</t>
+  </si>
+  <si>
+    <t>The screen real estate on this computer is a joy to behold. It's like having a panoramic view right on my desk. However, the lack of a physical webcam cover leaves me feeling uneasy about my privacy. I dream of the day when they introduce an automated privacy shutter that closes whenever the webcam is not in use.</t>
+  </si>
+  <si>
+    <t>The build quality of this computer is truly commendable, with a robust frame that feels like it can withstand a minor earthquake. However, the bland design leaves me yearning for more. If only they could introduce a customizable exterior that allows users to change the color and texture to suit their personal style!</t>
+  </si>
+  <si>
+    <t>The customer service for this computer was courteous and responsive when I had an issue. However, the long wait times on the phone were frustrating. I would be thrilled if they introduced a dedicated AI customer service assistant that could solve common issues instantly.</t>
+  </si>
+  <si>
+    <t>The 1080 resolution of the laptop feels as clear as my 27-inch 2K monitor, which I'm very satisfied with. If the computer screen could support 360-degree rotation, it would significantly enhance the user experience.</t>
+  </si>
+  <si>
+    <t>The computer's appearance is very exquisite, and the metallic texture is excellent. I suggest adding a waterproof function, with safe waterproofing within 10 meters, so you don't have to worry about the computer getting wet in extreme environments, at least not worrying about the situation where a water cup next to the computer spills.</t>
+  </si>
+  <si>
+    <t>The computer's cooling system is good, and it's compact and lightweight, suitable for business use. Business scenarios require extensive use of the call function, and if the computer could have a built-in SIM card, it would greatly improve business efficiency by being able to answer calls while using the computer.</t>
+  </si>
+  <si>
+    <t>The computer's touchpad is very sensitive, easy to operate, and easy to get used to. If there's room for optimization, I hope the touchpad can be a bit larger, acting as a digitizer. Using a stylus that comes with the computer, the touchpad can be used as a digitizer, so there's no need to carry an extra digitizer when doing design work, making the computer's functions more abundant.</t>
+  </si>
+  <si>
+    <t>The cost performance of the computer could be further improved; the price is too high, a few hundred dollars more expensive than those with equivalent configurations. It would be great if a laptop at this price could be configured with more than 10 graphics cards.</t>
+  </si>
+  <si>
+    <t>The computer is thin, light, and portable, with powerful functions, making it very suitable for business trips. One aspect that could be improved is the screen. The screen easily gets finger marks, whether from touching the screen with fingers or from the screen coming into contact with the keyboard when the lid is closed. It might be worth trying a non-fingerprint material for the screen.</t>
+  </si>
+  <si>
+    <t>The computer has no issues running games smoothly, and it feels like it won't have any problems for at least 3 years. The memory is also large, which can store a lot of things. In this case, I would want my computer to be more secure. I hope the computer can have a biometric function, recording my face, and verify it every time I boot up. If someone other than me peeks at my computer for a certain amount of time when I haven't locked it, it will send an alert to my phone and automatically lock the screen.</t>
+  </si>
+  <si>
+    <t>The laptop's sleek design is both aesthetically pleasing and practical. Its brushed metal finish lends a sense of luxury and durability. However, I'd love to see an anti-smudge coating to keep it looking clean and shiny.</t>
+  </si>
+  <si>
+    <t>I'm impressed by the crisp 1080p display, which provides a viewing experience akin to my high-resolution monitor at home. The option for a matte screen to reduce glare would be a fantastic addition for those of us who work in brightly lit environments.</t>
+  </si>
+  <si>
+    <t>This computer's battery life is exceptional, lasting the entire workday without needing a recharge. It would be incredible if future models incorporated solar charging capabilities for on-the-go use.</t>
+  </si>
+  <si>
+    <t>Its lightweight nature and slim profile make it the perfect travel companion. An in-built retractable privacy screen could further enhance its usability in public spaces.</t>
+  </si>
+  <si>
+    <t>The laptop's fast boot-up time is commendable. Imagine if it could learn from your usage patterns and pre-load frequently used applications upon startup - it would save so much time!</t>
+  </si>
+  <si>
+    <t>The cooling system is efficient, maintaining optimal performance during heavy-duty tasks. A silent operation mode for quieter environments would be a worthy addition.</t>
+  </si>
+  <si>
+    <t>The laptop's design is an exquisite blend of form and function, with a sleek profile that exudes elegance and a robust build that speaks of durability. I'm particularly fond of the metallic finish, which imparts a premium feel. Yet, I find myself constantly wiping off fingerprints to maintain its shine. An anti-smudge coating would be a game-changer.</t>
+  </si>
+  <si>
+    <t>The audio quality leaves a lot to be desired, especially when compared to the visual prowess of the 1080p display. The speakers lack richness and depth, which is disappointing for a device at this price point. An upgrade to a high-fidelity audio system would elevate the multimedia experience significantly.</t>
+  </si>
+  <si>
+    <t>Despite the laptop's slim form factor, it doesn't compromise on performance. It handles multiple applications with ease, delivering a seamless user experience. However, the fan noise during intensive tasks can be quite distracting, especially in quiet environments. An ultra-quiet cooling system would be a fantastic improvement.</t>
+  </si>
+  <si>
+    <t>The touchpad is a joy to use, responsive and smooth. However, the size leaves something to be desired. For professionals like me who often use the touchpad for design work, a larger surface area would mean fewer constraints and more freedom in our creative process.</t>
+  </si>
+  <si>
+    <t>I'm utterly frustrated with the laptop's battery life. For a device that boasts high performance, the battery drains faster than I would like. I find myself tethered to a power outlet more often than not. The inclusion of a higher capacity battery or a fast-charge feature would make this laptop truly mobile.</t>
+  </si>
+  <si>
+    <t>The laptop's security features are impressive, but they seem to lack that extra personal touch. Imagine a world where your laptop recognizes you, not just through a password or a fingerprint, but through your face, your voice, or even the way you type. That would truly revolutionize security and make it a far more personal, intimate experience.</t>
+  </si>
+  <si>
+    <t>The backlit keyboard is a godsend for late-night work sessions, but the lack of customization options is somewhat disappointing. The ability to adjust the color and brightness to suit one's mood or work environment would add a unique, personalized touch to the device.</t>
+  </si>
+  <si>
+    <t>It's disheartening to see such a high-quality laptop fall short in terms of storage options. With digital content becoming larger and more complex, the current storage options just don't cut it. A built-in expandable storage feature would be a welcome addition.</t>
+  </si>
+  <si>
+    <t>I find the laptop's webcam quality to be lackluster. In a time where virtual meetings have become the norm, a high-definition webcam is not just a luxury, but a necessity. An upgrade to a full HD webcam would significantly enhance video conferencing experiences.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
-      <name val="等线"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="9"/>
-      <name val="等线"/>
+      <name val="Calibri"/>
       <family val="3"/>
       <charset val="134"/>
       <scheme val="minor"/>
@@ -872,6 +1103,12 @@
     <font>
       <sz val="14"/>
       <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="16"/>
+      <color rgb="FF343541"/>
       <name val="Arial"/>
       <family val="2"/>
     </font>
@@ -911,16 +1148,17 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="常规" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -936,7 +1174,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 主题​​">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -1232,18 +1470,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E6697C36-D247-DE4E-9635-E653A91D407D}">
-  <dimension ref="A1:F81"/>
+  <dimension ref="A1:F82"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="93" workbookViewId="0">
-      <selection activeCell="F2" sqref="F2"/>
+    <sheetView tabSelected="1" topLeftCell="A62" zoomScale="93" workbookViewId="0">
+      <selection activeCell="F82" sqref="F82"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="16"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="123.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>6</v>
       </c>
@@ -1263,7 +1501,7 @@
         <v>266</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="20">
+    <row r="2" spans="1:6" ht="20" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>76</v>
       </c>
@@ -1279,8 +1517,11 @@
       <c r="E2" s="4" t="s">
         <v>105</v>
       </c>
-    </row>
-    <row r="3" spans="1:6" ht="20">
+      <c r="F2" s="6" t="s">
+        <v>267</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" ht="20" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
         <v>72</v>
       </c>
@@ -1296,8 +1537,11 @@
       <c r="E3" s="4" t="s">
         <v>106</v>
       </c>
-    </row>
-    <row r="4" spans="1:6" ht="20">
+      <c r="F3" s="6" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" ht="20" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
         <v>73</v>
       </c>
@@ -1313,8 +1557,11 @@
       <c r="E4" s="4" t="s">
         <v>107</v>
       </c>
-    </row>
-    <row r="5" spans="1:6" ht="20">
+      <c r="F4" s="4" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" ht="20" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
         <v>74</v>
       </c>
@@ -1330,8 +1577,11 @@
       <c r="E5" s="4" t="s">
         <v>108</v>
       </c>
-    </row>
-    <row r="6" spans="1:6" ht="20">
+      <c r="F5" s="4" t="s">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" ht="20" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
         <v>75</v>
       </c>
@@ -1347,8 +1597,11 @@
       <c r="E6" s="4" t="s">
         <v>109</v>
       </c>
-    </row>
-    <row r="7" spans="1:6" ht="20">
+      <c r="F6" s="4" t="s">
+        <v>271</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" ht="20" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
         <v>77</v>
       </c>
@@ -1364,8 +1617,11 @@
       <c r="E7" s="4" t="s">
         <v>110</v>
       </c>
-    </row>
-    <row r="8" spans="1:6" ht="20">
+      <c r="F7" s="4" t="s">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" ht="20" x14ac:dyDescent="0.2">
       <c r="A8" s="2" t="s">
         <v>78</v>
       </c>
@@ -1381,8 +1637,11 @@
       <c r="E8" s="4" t="s">
         <v>111</v>
       </c>
-    </row>
-    <row r="9" spans="1:6" ht="20">
+      <c r="F8" s="4" t="s">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" ht="20" x14ac:dyDescent="0.2">
       <c r="A9" s="2" t="s">
         <v>79</v>
       </c>
@@ -1398,8 +1657,11 @@
       <c r="E9" s="4" t="s">
         <v>112</v>
       </c>
-    </row>
-    <row r="10" spans="1:6" ht="20">
+      <c r="F9" s="4" t="s">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" ht="20" x14ac:dyDescent="0.2">
       <c r="A10" s="2" t="s">
         <v>80</v>
       </c>
@@ -1415,8 +1677,11 @@
       <c r="E10" s="4" t="s">
         <v>113</v>
       </c>
-    </row>
-    <row r="11" spans="1:6" ht="20">
+      <c r="F10" s="4" t="s">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" ht="20" x14ac:dyDescent="0.2">
       <c r="A11" s="2" t="s">
         <v>81</v>
       </c>
@@ -1432,8 +1697,11 @@
       <c r="E11" s="4" t="s">
         <v>114</v>
       </c>
-    </row>
-    <row r="12" spans="1:6" ht="20">
+      <c r="F11" s="4" t="s">
+        <v>276</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" ht="20" x14ac:dyDescent="0.2">
       <c r="A12" s="2" t="s">
         <v>82</v>
       </c>
@@ -1449,8 +1717,11 @@
       <c r="E12" s="4" t="s">
         <v>115</v>
       </c>
-    </row>
-    <row r="13" spans="1:6" ht="20">
+      <c r="F12" s="4" t="s">
+        <v>277</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" ht="20" x14ac:dyDescent="0.2">
       <c r="A13" s="2" t="s">
         <v>0</v>
       </c>
@@ -1466,8 +1737,11 @@
       <c r="E13" s="4" t="s">
         <v>116</v>
       </c>
-    </row>
-    <row r="14" spans="1:6" ht="20">
+      <c r="F13" s="4" t="s">
+        <v>278</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" ht="20" x14ac:dyDescent="0.2">
       <c r="A14" s="3" t="s">
         <v>1</v>
       </c>
@@ -1483,8 +1757,11 @@
       <c r="E14" s="4" t="s">
         <v>117</v>
       </c>
-    </row>
-    <row r="15" spans="1:6" ht="20">
+      <c r="F14" s="4" t="s">
+        <v>279</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" ht="20" x14ac:dyDescent="0.2">
       <c r="A15" s="1" t="s">
         <v>2</v>
       </c>
@@ -1500,8 +1777,11 @@
       <c r="E15" s="4" t="s">
         <v>118</v>
       </c>
-    </row>
-    <row r="16" spans="1:6" ht="20">
+      <c r="F15" s="4" t="s">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" ht="20" x14ac:dyDescent="0.2">
       <c r="A16" s="1" t="s">
         <v>3</v>
       </c>
@@ -1517,8 +1797,11 @@
       <c r="E16" s="4" t="s">
         <v>119</v>
       </c>
-    </row>
-    <row r="17" spans="1:5" ht="20">
+      <c r="F16" s="4" t="s">
+        <v>281</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" ht="20" x14ac:dyDescent="0.2">
       <c r="A17" s="1" t="s">
         <v>4</v>
       </c>
@@ -1534,8 +1817,11 @@
       <c r="E17" s="4" t="s">
         <v>120</v>
       </c>
-    </row>
-    <row r="18" spans="1:5" ht="20">
+      <c r="F17" s="4" t="s">
+        <v>282</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" ht="20" x14ac:dyDescent="0.2">
       <c r="A18" s="1" t="s">
         <v>5</v>
       </c>
@@ -1551,8 +1837,11 @@
       <c r="E18" s="4" t="s">
         <v>121</v>
       </c>
-    </row>
-    <row r="19" spans="1:5" ht="20">
+      <c r="F18" s="4" t="s">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" ht="20" x14ac:dyDescent="0.2">
       <c r="A19" s="1" t="s">
         <v>7</v>
       </c>
@@ -1568,8 +1857,11 @@
       <c r="E19" s="4" t="s">
         <v>122</v>
       </c>
-    </row>
-    <row r="20" spans="1:5" ht="20">
+      <c r="F19" s="4" t="s">
+        <v>284</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" ht="20" x14ac:dyDescent="0.2">
       <c r="A20" s="1" t="s">
         <v>8</v>
       </c>
@@ -1585,8 +1877,11 @@
       <c r="E20" s="4" t="s">
         <v>123</v>
       </c>
-    </row>
-    <row r="21" spans="1:5" ht="20">
+      <c r="F20" s="4" t="s">
+        <v>285</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" ht="20" x14ac:dyDescent="0.2">
       <c r="A21" s="1" t="s">
         <v>9</v>
       </c>
@@ -1602,8 +1897,11 @@
       <c r="E21" s="4" t="s">
         <v>124</v>
       </c>
-    </row>
-    <row r="22" spans="1:5" ht="20">
+      <c r="F21" s="4" t="s">
+        <v>286</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" ht="20" x14ac:dyDescent="0.2">
       <c r="A22" s="1" t="s">
         <v>10</v>
       </c>
@@ -1616,8 +1914,11 @@
       <c r="D22" s="4" t="s">
         <v>146</v>
       </c>
-    </row>
-    <row r="23" spans="1:5" ht="20">
+      <c r="F22" s="4" t="s">
+        <v>287</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" ht="20" x14ac:dyDescent="0.2">
       <c r="A23" s="1" t="s">
         <v>11</v>
       </c>
@@ -1630,8 +1931,11 @@
       <c r="D23" s="4" t="s">
         <v>147</v>
       </c>
-    </row>
-    <row r="24" spans="1:5" ht="20">
+      <c r="F23" s="4" t="s">
+        <v>288</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" ht="20" x14ac:dyDescent="0.2">
       <c r="A24" s="1" t="s">
         <v>12</v>
       </c>
@@ -1644,8 +1948,11 @@
       <c r="D24" s="4" t="s">
         <v>148</v>
       </c>
-    </row>
-    <row r="25" spans="1:5" ht="20">
+      <c r="F24" s="4" t="s">
+        <v>289</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" ht="20" x14ac:dyDescent="0.2">
       <c r="A25" s="1" t="s">
         <v>13</v>
       </c>
@@ -1658,8 +1965,11 @@
       <c r="D25" s="4" t="s">
         <v>149</v>
       </c>
-    </row>
-    <row r="26" spans="1:5" ht="20">
+      <c r="F25" s="4" t="s">
+        <v>290</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" ht="20" x14ac:dyDescent="0.2">
       <c r="A26" s="1" t="s">
         <v>14</v>
       </c>
@@ -1672,8 +1982,11 @@
       <c r="D26" s="4" t="s">
         <v>150</v>
       </c>
-    </row>
-    <row r="27" spans="1:5" ht="20">
+      <c r="F26" s="4" t="s">
+        <v>291</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" ht="20" x14ac:dyDescent="0.2">
       <c r="A27" s="1" t="s">
         <v>15</v>
       </c>
@@ -1686,8 +1999,11 @@
       <c r="D27" s="4" t="s">
         <v>151</v>
       </c>
-    </row>
-    <row r="28" spans="1:5" ht="20">
+      <c r="F27" s="4" t="s">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" ht="20" x14ac:dyDescent="0.2">
       <c r="A28" s="1" t="s">
         <v>16</v>
       </c>
@@ -1700,8 +2016,11 @@
       <c r="D28" s="4" t="s">
         <v>152</v>
       </c>
-    </row>
-    <row r="29" spans="1:5" ht="20">
+      <c r="F28" s="4" t="s">
+        <v>293</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" ht="20" x14ac:dyDescent="0.2">
       <c r="A29" s="1" t="s">
         <v>17</v>
       </c>
@@ -1714,8 +2033,11 @@
       <c r="D29" s="4" t="s">
         <v>153</v>
       </c>
-    </row>
-    <row r="30" spans="1:5" ht="20">
+      <c r="F29" s="4" t="s">
+        <v>294</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" ht="20" x14ac:dyDescent="0.2">
       <c r="A30" s="1" t="s">
         <v>18</v>
       </c>
@@ -1728,8 +2050,11 @@
       <c r="D30" s="4" t="s">
         <v>154</v>
       </c>
-    </row>
-    <row r="31" spans="1:5" ht="20">
+      <c r="F30" s="4" t="s">
+        <v>295</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" ht="20" x14ac:dyDescent="0.2">
       <c r="A31" s="1" t="s">
         <v>19</v>
       </c>
@@ -1742,8 +2067,11 @@
       <c r="D31" s="4" t="s">
         <v>155</v>
       </c>
-    </row>
-    <row r="32" spans="1:5" ht="20">
+      <c r="F31" s="4" t="s">
+        <v>296</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" ht="20" x14ac:dyDescent="0.2">
       <c r="A32" s="1" t="s">
         <v>20</v>
       </c>
@@ -1756,8 +2084,11 @@
       <c r="D32" s="4" t="s">
         <v>156</v>
       </c>
-    </row>
-    <row r="33" spans="1:4" ht="20">
+      <c r="F32" s="4" t="s">
+        <v>297</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" ht="20" x14ac:dyDescent="0.2">
       <c r="A33" s="1" t="s">
         <v>21</v>
       </c>
@@ -1770,8 +2101,11 @@
       <c r="D33" s="4" t="s">
         <v>157</v>
       </c>
-    </row>
-    <row r="34" spans="1:4" ht="20">
+      <c r="F33" s="4" t="s">
+        <v>298</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" ht="20" x14ac:dyDescent="0.2">
       <c r="A34" s="1" t="s">
         <v>22</v>
       </c>
@@ -1784,8 +2118,11 @@
       <c r="D34" s="4" t="s">
         <v>158</v>
       </c>
-    </row>
-    <row r="35" spans="1:4" ht="20">
+      <c r="F34" s="4" t="s">
+        <v>299</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" ht="20" x14ac:dyDescent="0.2">
       <c r="A35" s="1" t="s">
         <v>23</v>
       </c>
@@ -1798,8 +2135,11 @@
       <c r="D35" s="4" t="s">
         <v>159</v>
       </c>
-    </row>
-    <row r="36" spans="1:4" ht="20">
+      <c r="F35" s="4" t="s">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" ht="20" x14ac:dyDescent="0.2">
       <c r="A36" s="1" t="s">
         <v>24</v>
       </c>
@@ -1812,8 +2152,11 @@
       <c r="D36" s="4" t="s">
         <v>160</v>
       </c>
-    </row>
-    <row r="37" spans="1:4" ht="20">
+      <c r="F36" s="4" t="s">
+        <v>301</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6" ht="20" x14ac:dyDescent="0.2">
       <c r="A37" s="1" t="s">
         <v>25</v>
       </c>
@@ -1826,8 +2169,11 @@
       <c r="D37" s="4" t="s">
         <v>161</v>
       </c>
-    </row>
-    <row r="38" spans="1:4" ht="20">
+      <c r="F37" s="4" t="s">
+        <v>302</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6" ht="20" x14ac:dyDescent="0.2">
       <c r="A38" s="1" t="s">
         <v>26</v>
       </c>
@@ -1840,8 +2186,11 @@
       <c r="D38" s="4" t="s">
         <v>162</v>
       </c>
-    </row>
-    <row r="39" spans="1:4" ht="20">
+      <c r="F38" s="4" t="s">
+        <v>303</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6" ht="20" x14ac:dyDescent="0.2">
       <c r="A39" s="1" t="s">
         <v>27</v>
       </c>
@@ -1854,8 +2203,11 @@
       <c r="D39" s="4" t="s">
         <v>163</v>
       </c>
-    </row>
-    <row r="40" spans="1:4" ht="20">
+      <c r="F39" s="4" t="s">
+        <v>304</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6" ht="20" x14ac:dyDescent="0.2">
       <c r="A40" s="1" t="s">
         <v>28</v>
       </c>
@@ -1868,8 +2220,11 @@
       <c r="D40" s="4" t="s">
         <v>164</v>
       </c>
-    </row>
-    <row r="41" spans="1:4" ht="20">
+      <c r="F40" s="4" t="s">
+        <v>305</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6" ht="20" x14ac:dyDescent="0.2">
       <c r="A41" s="1" t="s">
         <v>29</v>
       </c>
@@ -1882,8 +2237,11 @@
       <c r="D41" s="4" t="s">
         <v>165</v>
       </c>
-    </row>
-    <row r="42" spans="1:4" ht="20">
+      <c r="F41" s="4" t="s">
+        <v>306</v>
+      </c>
+    </row>
+    <row r="42" spans="1:6" ht="20" x14ac:dyDescent="0.2">
       <c r="A42" s="1" t="s">
         <v>30</v>
       </c>
@@ -1896,8 +2254,11 @@
       <c r="D42" s="4" t="s">
         <v>226</v>
       </c>
-    </row>
-    <row r="43" spans="1:4" ht="20">
+      <c r="F42" s="4" t="s">
+        <v>307</v>
+      </c>
+    </row>
+    <row r="43" spans="1:6" ht="20" x14ac:dyDescent="0.2">
       <c r="A43" s="1" t="s">
         <v>31</v>
       </c>
@@ -1910,8 +2271,11 @@
       <c r="D43" s="4" t="s">
         <v>227</v>
       </c>
-    </row>
-    <row r="44" spans="1:4" ht="20">
+      <c r="F43" s="4" t="s">
+        <v>308</v>
+      </c>
+    </row>
+    <row r="44" spans="1:6" ht="20" x14ac:dyDescent="0.2">
       <c r="A44" s="1" t="s">
         <v>32</v>
       </c>
@@ -1924,8 +2288,11 @@
       <c r="D44" s="4" t="s">
         <v>228</v>
       </c>
-    </row>
-    <row r="45" spans="1:4" ht="20">
+      <c r="F44" s="4" t="s">
+        <v>309</v>
+      </c>
+    </row>
+    <row r="45" spans="1:6" ht="20" x14ac:dyDescent="0.2">
       <c r="A45" s="1" t="s">
         <v>33</v>
       </c>
@@ -1938,8 +2305,11 @@
       <c r="D45" s="4" t="s">
         <v>229</v>
       </c>
-    </row>
-    <row r="46" spans="1:4" ht="20">
+      <c r="F45" s="4" t="s">
+        <v>310</v>
+      </c>
+    </row>
+    <row r="46" spans="1:6" ht="20" x14ac:dyDescent="0.2">
       <c r="A46" s="1" t="s">
         <v>34</v>
       </c>
@@ -1952,8 +2322,11 @@
       <c r="D46" s="4" t="s">
         <v>230</v>
       </c>
-    </row>
-    <row r="47" spans="1:4" ht="20">
+      <c r="F46" s="4" t="s">
+        <v>311</v>
+      </c>
+    </row>
+    <row r="47" spans="1:6" ht="20" x14ac:dyDescent="0.2">
       <c r="A47" s="1" t="s">
         <v>35</v>
       </c>
@@ -1966,8 +2339,11 @@
       <c r="D47" s="4" t="s">
         <v>231</v>
       </c>
-    </row>
-    <row r="48" spans="1:4" ht="20">
+      <c r="F47" s="4" t="s">
+        <v>312</v>
+      </c>
+    </row>
+    <row r="48" spans="1:6" ht="20" x14ac:dyDescent="0.2">
       <c r="A48" s="1" t="s">
         <v>36</v>
       </c>
@@ -1980,8 +2356,11 @@
       <c r="D48" s="4" t="s">
         <v>232</v>
       </c>
-    </row>
-    <row r="49" spans="1:4" ht="20">
+      <c r="F48" s="4" t="s">
+        <v>313</v>
+      </c>
+    </row>
+    <row r="49" spans="1:6" ht="20" x14ac:dyDescent="0.2">
       <c r="A49" s="1" t="s">
         <v>37</v>
       </c>
@@ -1994,8 +2373,11 @@
       <c r="D49" s="4" t="s">
         <v>233</v>
       </c>
-    </row>
-    <row r="50" spans="1:4" ht="20">
+      <c r="F49" s="4" t="s">
+        <v>314</v>
+      </c>
+    </row>
+    <row r="50" spans="1:6" ht="20" x14ac:dyDescent="0.2">
       <c r="A50" s="1" t="s">
         <v>38</v>
       </c>
@@ -2008,8 +2390,11 @@
       <c r="D50" s="4" t="s">
         <v>234</v>
       </c>
-    </row>
-    <row r="51" spans="1:4" ht="20">
+      <c r="F50" s="4" t="s">
+        <v>315</v>
+      </c>
+    </row>
+    <row r="51" spans="1:6" ht="20" x14ac:dyDescent="0.2">
       <c r="A51" s="1" t="s">
         <v>39</v>
       </c>
@@ -2022,8 +2407,11 @@
       <c r="D51" s="4" t="s">
         <v>235</v>
       </c>
-    </row>
-    <row r="52" spans="1:4" ht="20">
+      <c r="F51" s="4" t="s">
+        <v>316</v>
+      </c>
+    </row>
+    <row r="52" spans="1:6" ht="20" x14ac:dyDescent="0.2">
       <c r="A52" s="1" t="s">
         <v>40</v>
       </c>
@@ -2036,8 +2424,11 @@
       <c r="D52" s="4" t="s">
         <v>236</v>
       </c>
-    </row>
-    <row r="53" spans="1:4" ht="20">
+      <c r="F52" s="4" t="s">
+        <v>317</v>
+      </c>
+    </row>
+    <row r="53" spans="1:6" ht="20" x14ac:dyDescent="0.2">
       <c r="A53" s="1" t="s">
         <v>41</v>
       </c>
@@ -2050,8 +2441,11 @@
       <c r="D53" s="4" t="s">
         <v>237</v>
       </c>
-    </row>
-    <row r="54" spans="1:4" ht="20">
+      <c r="F53" s="4" t="s">
+        <v>318</v>
+      </c>
+    </row>
+    <row r="54" spans="1:6" ht="20" x14ac:dyDescent="0.2">
       <c r="A54" s="1" t="s">
         <v>42</v>
       </c>
@@ -2064,8 +2458,11 @@
       <c r="D54" s="4" t="s">
         <v>238</v>
       </c>
-    </row>
-    <row r="55" spans="1:4" ht="20">
+      <c r="F54" s="4" t="s">
+        <v>319</v>
+      </c>
+    </row>
+    <row r="55" spans="1:6" ht="20" x14ac:dyDescent="0.2">
       <c r="A55" s="1" t="s">
         <v>43</v>
       </c>
@@ -2078,8 +2475,11 @@
       <c r="D55" s="4" t="s">
         <v>239</v>
       </c>
-    </row>
-    <row r="56" spans="1:4" ht="20">
+      <c r="F55" s="4" t="s">
+        <v>320</v>
+      </c>
+    </row>
+    <row r="56" spans="1:6" ht="20" x14ac:dyDescent="0.2">
       <c r="A56" s="1" t="s">
         <v>44</v>
       </c>
@@ -2092,8 +2492,11 @@
       <c r="D56" s="4" t="s">
         <v>240</v>
       </c>
-    </row>
-    <row r="57" spans="1:4" ht="20">
+      <c r="F56" s="4" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="57" spans="1:6" ht="20" x14ac:dyDescent="0.2">
       <c r="A57" s="1" t="s">
         <v>45</v>
       </c>
@@ -2106,8 +2509,11 @@
       <c r="D57" s="4" t="s">
         <v>241</v>
       </c>
-    </row>
-    <row r="58" spans="1:4" ht="20">
+      <c r="F57" s="4" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="58" spans="1:6" ht="20" x14ac:dyDescent="0.2">
       <c r="A58" s="1" t="s">
         <v>46</v>
       </c>
@@ -2120,8 +2526,11 @@
       <c r="D58" s="4" t="s">
         <v>242</v>
       </c>
-    </row>
-    <row r="59" spans="1:4" ht="20">
+      <c r="F58" s="4" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="59" spans="1:6" ht="20" x14ac:dyDescent="0.2">
       <c r="A59" s="1" t="s">
         <v>47</v>
       </c>
@@ -2134,8 +2543,11 @@
       <c r="D59" s="4" t="s">
         <v>243</v>
       </c>
-    </row>
-    <row r="60" spans="1:4" ht="20">
+      <c r="F59" s="4" t="s">
+        <v>321</v>
+      </c>
+    </row>
+    <row r="60" spans="1:6" ht="20" x14ac:dyDescent="0.2">
       <c r="A60" s="1" t="s">
         <v>48</v>
       </c>
@@ -2148,8 +2560,11 @@
       <c r="D60" s="4" t="s">
         <v>244</v>
       </c>
-    </row>
-    <row r="61" spans="1:4" ht="20">
+      <c r="F60" s="4" t="s">
+        <v>322</v>
+      </c>
+    </row>
+    <row r="61" spans="1:6" ht="20" x14ac:dyDescent="0.2">
       <c r="A61" s="1" t="s">
         <v>49</v>
       </c>
@@ -2162,8 +2577,11 @@
       <c r="D61" s="4" t="s">
         <v>245</v>
       </c>
-    </row>
-    <row r="62" spans="1:4" ht="20">
+      <c r="F61" s="4" t="s">
+        <v>323</v>
+      </c>
+    </row>
+    <row r="62" spans="1:6" ht="20" x14ac:dyDescent="0.2">
       <c r="A62" s="1" t="s">
         <v>50</v>
       </c>
@@ -2176,8 +2594,11 @@
       <c r="D62" s="5" t="s">
         <v>246</v>
       </c>
-    </row>
-    <row r="63" spans="1:4" ht="20">
+      <c r="F62" s="4" t="s">
+        <v>324</v>
+      </c>
+    </row>
+    <row r="63" spans="1:6" ht="20" x14ac:dyDescent="0.2">
       <c r="A63" s="1" t="s">
         <v>51</v>
       </c>
@@ -2190,8 +2611,11 @@
       <c r="D63" s="5" t="s">
         <v>247</v>
       </c>
-    </row>
-    <row r="64" spans="1:4" ht="20">
+      <c r="F63" s="4" t="s">
+        <v>325</v>
+      </c>
+    </row>
+    <row r="64" spans="1:6" ht="20" x14ac:dyDescent="0.2">
       <c r="A64" s="1" t="s">
         <v>52</v>
       </c>
@@ -2204,8 +2628,11 @@
       <c r="D64" s="5" t="s">
         <v>248</v>
       </c>
-    </row>
-    <row r="65" spans="1:4" ht="20">
+      <c r="F64" s="4" t="s">
+        <v>326</v>
+      </c>
+    </row>
+    <row r="65" spans="1:6" ht="20" x14ac:dyDescent="0.2">
       <c r="A65" s="1" t="s">
         <v>53</v>
       </c>
@@ -2218,8 +2645,11 @@
       <c r="D65" s="5" t="s">
         <v>249</v>
       </c>
-    </row>
-    <row r="66" spans="1:4" ht="20">
+      <c r="F65" s="4" t="s">
+        <v>327</v>
+      </c>
+    </row>
+    <row r="66" spans="1:6" ht="20" x14ac:dyDescent="0.2">
       <c r="A66" s="1" t="s">
         <v>54</v>
       </c>
@@ -2232,8 +2662,11 @@
       <c r="D66" s="5" t="s">
         <v>250</v>
       </c>
-    </row>
-    <row r="67" spans="1:4" ht="20">
+      <c r="F66" s="4" t="s">
+        <v>328</v>
+      </c>
+    </row>
+    <row r="67" spans="1:6" ht="20" x14ac:dyDescent="0.2">
       <c r="A67" s="1" t="s">
         <v>55</v>
       </c>
@@ -2246,8 +2679,11 @@
       <c r="D67" s="5" t="s">
         <v>251</v>
       </c>
-    </row>
-    <row r="68" spans="1:4" ht="20">
+      <c r="F67" s="4" t="s">
+        <v>329</v>
+      </c>
+    </row>
+    <row r="68" spans="1:6" ht="20" x14ac:dyDescent="0.2">
       <c r="A68" s="1" t="s">
         <v>56</v>
       </c>
@@ -2260,8 +2696,11 @@
       <c r="D68" s="5" t="s">
         <v>252</v>
       </c>
-    </row>
-    <row r="69" spans="1:4" ht="20">
+      <c r="F68" s="4" t="s">
+        <v>330</v>
+      </c>
+    </row>
+    <row r="69" spans="1:6" ht="20" x14ac:dyDescent="0.2">
       <c r="A69" s="1" t="s">
         <v>57</v>
       </c>
@@ -2274,8 +2713,11 @@
       <c r="D69" s="5" t="s">
         <v>253</v>
       </c>
-    </row>
-    <row r="70" spans="1:4" ht="20">
+      <c r="F69" s="4" t="s">
+        <v>331</v>
+      </c>
+    </row>
+    <row r="70" spans="1:6" ht="20" x14ac:dyDescent="0.2">
       <c r="A70" s="1" t="s">
         <v>58</v>
       </c>
@@ -2288,8 +2730,11 @@
       <c r="D70" s="5" t="s">
         <v>254</v>
       </c>
-    </row>
-    <row r="71" spans="1:4" ht="20">
+      <c r="F70" s="4" t="s">
+        <v>332</v>
+      </c>
+    </row>
+    <row r="71" spans="1:6" ht="20" x14ac:dyDescent="0.2">
       <c r="A71" s="1" t="s">
         <v>59</v>
       </c>
@@ -2302,8 +2747,11 @@
       <c r="D71" s="5" t="s">
         <v>255</v>
       </c>
-    </row>
-    <row r="72" spans="1:4" ht="20">
+      <c r="F71" s="4" t="s">
+        <v>333</v>
+      </c>
+    </row>
+    <row r="72" spans="1:6" ht="20" x14ac:dyDescent="0.2">
       <c r="A72" s="1" t="s">
         <v>60</v>
       </c>
@@ -2316,8 +2764,11 @@
       <c r="D72" s="5" t="s">
         <v>256</v>
       </c>
-    </row>
-    <row r="73" spans="1:4" ht="20">
+      <c r="F72" s="4" t="s">
+        <v>334</v>
+      </c>
+    </row>
+    <row r="73" spans="1:6" ht="20" x14ac:dyDescent="0.2">
       <c r="A73" s="1" t="s">
         <v>61</v>
       </c>
@@ -2330,8 +2781,11 @@
       <c r="D73" s="5" t="s">
         <v>257</v>
       </c>
-    </row>
-    <row r="74" spans="1:4" ht="20">
+      <c r="F73" s="4" t="s">
+        <v>335</v>
+      </c>
+    </row>
+    <row r="74" spans="1:6" ht="20" x14ac:dyDescent="0.2">
       <c r="A74" s="1" t="s">
         <v>62</v>
       </c>
@@ -2344,8 +2798,11 @@
       <c r="D74" s="5" t="s">
         <v>258</v>
       </c>
-    </row>
-    <row r="75" spans="1:4" ht="20">
+      <c r="F74" s="4" t="s">
+        <v>336</v>
+      </c>
+    </row>
+    <row r="75" spans="1:6" ht="20" x14ac:dyDescent="0.2">
       <c r="A75" s="1" t="s">
         <v>63</v>
       </c>
@@ -2358,8 +2815,11 @@
       <c r="D75" s="5" t="s">
         <v>259</v>
       </c>
-    </row>
-    <row r="76" spans="1:4" ht="20">
+      <c r="F75" s="4" t="s">
+        <v>337</v>
+      </c>
+    </row>
+    <row r="76" spans="1:6" ht="20" x14ac:dyDescent="0.2">
       <c r="A76" s="1" t="s">
         <v>64</v>
       </c>
@@ -2372,8 +2832,11 @@
       <c r="D76" s="5" t="s">
         <v>260</v>
       </c>
-    </row>
-    <row r="77" spans="1:4" ht="20">
+      <c r="F76" s="4" t="s">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="77" spans="1:6" ht="20" x14ac:dyDescent="0.2">
       <c r="A77" s="1" t="s">
         <v>65</v>
       </c>
@@ -2386,8 +2849,11 @@
       <c r="D77" s="5" t="s">
         <v>261</v>
       </c>
-    </row>
-    <row r="78" spans="1:4" ht="20">
+      <c r="F77" s="4" t="s">
+        <v>339</v>
+      </c>
+    </row>
+    <row r="78" spans="1:6" ht="20" x14ac:dyDescent="0.2">
       <c r="A78" s="1" t="s">
         <v>66</v>
       </c>
@@ -2400,8 +2866,11 @@
       <c r="D78" s="5" t="s">
         <v>262</v>
       </c>
-    </row>
-    <row r="79" spans="1:4" ht="20">
+      <c r="F78" s="4" t="s">
+        <v>340</v>
+      </c>
+    </row>
+    <row r="79" spans="1:6" ht="20" x14ac:dyDescent="0.2">
       <c r="A79" s="1" t="s">
         <v>67</v>
       </c>
@@ -2414,8 +2883,11 @@
       <c r="D79" s="5" t="s">
         <v>263</v>
       </c>
-    </row>
-    <row r="80" spans="1:4" ht="20">
+      <c r="F79" s="4" t="s">
+        <v>341</v>
+      </c>
+    </row>
+    <row r="80" spans="1:6" ht="20" x14ac:dyDescent="0.2">
       <c r="A80" s="1" t="s">
         <v>68</v>
       </c>
@@ -2428,8 +2900,11 @@
       <c r="D80" s="5" t="s">
         <v>264</v>
       </c>
-    </row>
-    <row r="81" spans="1:4" ht="20">
+      <c r="F80" s="4" t="s">
+        <v>342</v>
+      </c>
+    </row>
+    <row r="81" spans="1:6" ht="20" x14ac:dyDescent="0.2">
       <c r="A81" s="1" t="s">
         <v>69</v>
       </c>
@@ -2442,6 +2917,12 @@
       <c r="D81" s="5" t="s">
         <v>265</v>
       </c>
+      <c r="F81" s="4" t="s">
+        <v>343</v>
+      </c>
+    </row>
+    <row r="82" spans="1:6" ht="20" x14ac:dyDescent="0.2">
+      <c r="F82" s="4"/>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>

</xml_diff>